<commit_message>
added org update and delete test case
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -21,18 +21,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>AUTO_ORG_l</t>
   </si>
   <si>
     <t>OrgName</t>
   </si>
+  <si>
+    <t>AUTO_ORG_ERZYN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XEV4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -387,7 +391,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="16376" max="16384" width="11.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="16376" max="16384" customWidth="true" style="1" width="11.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -396,9 +400,9 @@
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added sub org add test case
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CD7F34B1-C529-40DA-9E5E-548C60647B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{649A5E78-A3E8-47BC-B6E1-A699E1A780FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="16450" windowHeight="11060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="16490" windowHeight="11060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,54 +21,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>AUTO_ORG_l</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>OrgName</t>
   </si>
   <si>
-    <t>AUTO_ORG_ERZYN</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_VBOFK</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_FFZMJ</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_KVZQW</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_NVKVN</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_UFNCV</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_USPHR</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_FEKYV</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_BXQIY</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_AHDID</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_BCFRL</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_XWQFZ</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_TZBDH</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_VPMVD</t>
+    <t>AUTO_ORG_URIUT</t>
+  </si>
+  <si>
+    <t>SubOrgName</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_ZSVGP</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_QHYKH</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_TJLKG</t>
   </si>
 </sst>
 </file>
@@ -425,7 +395,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,13 +405,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>15</v>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added sub org add test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{649A5E78-A3E8-47BC-B6E1-A699E1A780FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{760B55F0-78F7-4709-8EFE-FC4D81D1C96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="16490" windowHeight="11060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="16530" windowHeight="11060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="OrgData" sheetId="1" r:id="rId1"/>
+    <sheet name="SubOrgData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:N5"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,24 +22,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>OrgName</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_URIUT</t>
   </si>
   <si>
     <t>SubOrgName</t>
   </si>
   <si>
-    <t>AUTO_SUB_ORG_ZSVGP</t>
+    <t>AUTO_SUB_ORG_IUWXW</t>
   </si>
   <si>
-    <t>AUTO_ORG_QHYKH</t>
+    <t>AUTO_ORG_GQNCW</t>
   </si>
   <si>
-    <t>AUTO_SUB_ORG_TJLKG</t>
+    <t>AUTO_SUB_ORG_UQAXU</t>
   </si>
 </sst>
 </file>
@@ -392,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -407,13 +405,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
-      <c r="B2" t="s">
-        <v>5</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35"/>
@@ -422,4 +417,29 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660B5572-4ACD-44A0-9082-FDAA1F80183F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modify sub org script
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>OrgName</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>AUTO_SUB_ORG_UQAXU</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_PAVNO</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_ESVEA</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35"/>
@@ -436,7 +442,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added edit sub org test case
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>OrgName</t>
   </si>
@@ -43,6 +43,24 @@
   </si>
   <si>
     <t>AUTO_SUB_ORG_ESVEA</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_EKKKG</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_GTZUI</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_ICREV</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_LBTPX</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_QULEZ</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_MQUCV</t>
   </si>
 </sst>
 </file>
@@ -442,7 +460,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify add member scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>OrgName</t>
   </si>
@@ -38,12 +38,34 @@
   </si>
   <si>
     <t>MemberName</t>
+  </si>
+  <si>
+    <t>First6376</t>
+  </si>
+  <si>
+    <t>First9937</t>
+  </si>
+  <si>
+    <t>First3176</t>
+  </si>
+  <si>
+    <t>First7970</t>
+  </si>
+  <si>
+    <t>First2407</t>
+  </si>
+  <si>
+    <t>First9118</t>
+  </si>
+  <si>
+    <t>First9668</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XEV4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B2"/>
@@ -398,7 +420,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="16376" max="16384" width="11.54296875" style="1" customWidth="1" collapsed="1"/>
+    <col min="16376" max="16384" customWidth="true" style="1" width="11.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -444,7 +466,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A56F17-F556-4737-8271-EB2D7316592D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -457,6 +479,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added member testcase edit delete
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>OrgName</t>
   </si>
@@ -59,6 +59,180 @@
   </si>
   <si>
     <t>First9668</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_WASQX</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_JSPXS</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_JLLXE</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_PXIYC</t>
+  </si>
+  <si>
+    <t>First8853</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_QMRUD</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_PJQTH</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_WTKWQ</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_ZRYHN</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_SKYZC</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_DQUJE</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_MMJTB</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_HZBTA</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_ZWTPM</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_OFSDM</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_BWDAT</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_KEJKP</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_ZLSLD</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_SXMKX</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_RUATB</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_XFLXL</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_XXKWN</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_WRTVV</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_TYLCC</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_SIBZJ</t>
+  </si>
+  <si>
+    <t>First1086</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_RKFOC</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_ZDCIR</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_CYIDR</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_UCHKL</t>
+  </si>
+  <si>
+    <t>First9342</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_MCHLK</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_RHIOI</t>
+  </si>
+  <si>
+    <t>First2021</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_NXXTE</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_XDNLR</t>
+  </si>
+  <si>
+    <t>First6994</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_VVCSX</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_RPVUZ</t>
+  </si>
+  <si>
+    <t>First3131</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_TVRNH</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_AWAGE</t>
+  </si>
+  <si>
+    <t>First1754</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_NJZYC</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_UAYNL</t>
+  </si>
+  <si>
+    <t>First1753</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_UVHKC</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_RNZRC</t>
+  </si>
+  <si>
+    <t>First3999</t>
+  </si>
+  <si>
+    <t>First703</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_RAXMF</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_FJOYX</t>
+  </si>
+  <si>
+    <t>First5954</t>
+  </si>
+  <si>
+    <t>First6947</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_HCDAJ</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_YMKWH</t>
+  </si>
+  <si>
+    <t>First76</t>
+  </si>
+  <si>
+    <t>First9290</t>
   </si>
 </sst>
 </file>
@@ -428,9 +602,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35"/>
@@ -454,9 +628,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -481,7 +655,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified script according to new change
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>OrgName</t>
   </si>
@@ -81,6 +81,69 @@
   </si>
   <si>
     <t>SFirstJPCFG</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_MHUXC</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_RMMXU</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_KCARI</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_ETOGY</t>
+  </si>
+  <si>
+    <t>First1309</t>
+  </si>
+  <si>
+    <t>SFirstVDGAD</t>
+  </si>
+  <si>
+    <t>SFirstCXAQK</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_VETHF</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_AKGCL</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_AIAKB</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_RPCQB</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_QZOZU</t>
+  </si>
+  <si>
+    <t>First6156</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_ESYDR</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_EMWRC</t>
+  </si>
+  <si>
+    <t>AUTO_SUB_ORG_CSNPH</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_RBLQH</t>
+  </si>
+  <si>
+    <t>First8290</t>
+  </si>
+  <si>
+    <t>First6563</t>
+  </si>
+  <si>
+    <t>SFirstRSUHZ</t>
+  </si>
+  <si>
+    <t>SFirstWSOPJ</t>
   </si>
 </sst>
 </file>
@@ -452,7 +515,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35"/>
@@ -478,7 +541,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -501,7 +564,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -526,7 +589,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added delete bulk with multi records scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>OrgName</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>SFirstWSOPJ</t>
+  </si>
+  <si>
+    <t>AUTO_ORG_CNFOY</t>
   </si>
 </sst>
 </file>
@@ -515,7 +518,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added gen report test case
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>OrgName</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>AUTO_ORG_CNFOY</t>
+  </si>
+  <si>
+    <t>First2095</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added delete  confirm message scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>OrgName</t>
   </si>
@@ -150,6 +150,51 @@
   </si>
   <si>
     <t>First2095</t>
+  </si>
+  <si>
+    <t>SFirstITMDV</t>
+  </si>
+  <si>
+    <t>SFirstGCLMP</t>
+  </si>
+  <si>
+    <t>SFirstEGEGR</t>
+  </si>
+  <si>
+    <t>SFirstOXPHJ</t>
+  </si>
+  <si>
+    <t>SFirstHTYWP</t>
+  </si>
+  <si>
+    <t>SFirstGUSYS</t>
+  </si>
+  <si>
+    <t>SFirstXUVGK</t>
+  </si>
+  <si>
+    <t>SFirstIEAXV</t>
+  </si>
+  <si>
+    <t>SLastVZYCF</t>
+  </si>
+  <si>
+    <t>SFirstHCYLE</t>
+  </si>
+  <si>
+    <t>SLastAVLAF</t>
+  </si>
+  <si>
+    <t>SFirstNEIAM</t>
+  </si>
+  <si>
+    <t>SLastYPLPU</t>
+  </si>
+  <si>
+    <t>SFirstLRZST</t>
+  </si>
+  <si>
+    <t>SLastVSAHI</t>
   </si>
 </sst>
 </file>
@@ -580,7 +625,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74720F76-F09E-4599-AA7C-379CD9963F54}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -595,7 +640,12 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added prompt add scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{379D57BD-8ED2-40A4-9BDC-83B2223BA100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{27E43E09-A175-43B3-9CBC-A575CB3726B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="16610" windowHeight="11060" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrgData" sheetId="1" r:id="rId1"/>
     <sheet name="SubOrgData" sheetId="2" r:id="rId2"/>
     <sheet name="MemberData" sheetId="3" r:id="rId3"/>
     <sheet name="StaffData" sheetId="4" r:id="rId4"/>
+    <sheet name="prompt" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A1:N6"/>
+  <oleSize ref="A1:N5"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>OrgName</t>
   </si>
@@ -35,166 +36,25 @@
     <t>MemberName</t>
   </si>
   <si>
-    <t>AUTO_ORG_GPMCY</t>
-  </si>
-  <si>
-    <t>AUTO_SUB_ORG_WQBXK</t>
-  </si>
-  <si>
-    <t>First9115</t>
-  </si>
-  <si>
     <t>StaffName</t>
   </si>
   <si>
-    <t>STaffFirst6343</t>
-  </si>
-  <si>
-    <t>STaffFirst8104</t>
-  </si>
-  <si>
-    <t>STaffFirstFIOSW</t>
-  </si>
-  <si>
-    <t>SFirstNAPVJ</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_KFQZK</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_IETIQ</t>
-  </si>
-  <si>
-    <t>AUTO_SUB_ORG_ANNAL</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_YZRPW</t>
-  </si>
-  <si>
-    <t>First1977</t>
-  </si>
-  <si>
-    <t>First4108</t>
-  </si>
-  <si>
-    <t>SFirstOZNXU</t>
-  </si>
-  <si>
-    <t>SFirstJPCFG</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_MHUXC</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_RMMXU</t>
-  </si>
-  <si>
-    <t>AUTO_SUB_ORG_KCARI</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_ETOGY</t>
-  </si>
-  <si>
-    <t>First1309</t>
-  </si>
-  <si>
-    <t>SFirstVDGAD</t>
-  </si>
-  <si>
-    <t>SFirstCXAQK</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_VETHF</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_AKGCL</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_AIAKB</t>
-  </si>
-  <si>
-    <t>AUTO_SUB_ORG_RPCQB</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_QZOZU</t>
-  </si>
-  <si>
-    <t>First6156</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_ESYDR</t>
-  </si>
-  <si>
-    <t>AUTO_ORG_EMWRC</t>
-  </si>
-  <si>
-    <t>AUTO_SUB_ORG_CSNPH</t>
-  </si>
-  <si>
     <t>AUTO_ORG_RBLQH</t>
   </si>
   <si>
-    <t>First8290</t>
-  </si>
-  <si>
-    <t>First6563</t>
-  </si>
-  <si>
-    <t>SFirstRSUHZ</t>
-  </si>
-  <si>
-    <t>SFirstWSOPJ</t>
-  </si>
-  <si>
     <t>AUTO_ORG_CNFOY</t>
   </si>
   <si>
     <t>First2095</t>
   </si>
   <si>
-    <t>SFirstITMDV</t>
-  </si>
-  <si>
-    <t>SFirstGCLMP</t>
-  </si>
-  <si>
-    <t>SFirstEGEGR</t>
-  </si>
-  <si>
-    <t>SFirstOXPHJ</t>
-  </si>
-  <si>
-    <t>SFirstHTYWP</t>
-  </si>
-  <si>
-    <t>SFirstGUSYS</t>
-  </si>
-  <si>
-    <t>SFirstXUVGK</t>
-  </si>
-  <si>
-    <t>SFirstIEAXV</t>
-  </si>
-  <si>
-    <t>SLastVZYCF</t>
-  </si>
-  <si>
-    <t>SFirstHCYLE</t>
-  </si>
-  <si>
-    <t>SLastAVLAF</t>
-  </si>
-  <si>
-    <t>SFirstNEIAM</t>
-  </si>
-  <si>
-    <t>SLastYPLPU</t>
-  </si>
-  <si>
     <t>SFirstLRZST</t>
   </si>
   <si>
     <t>SLastVSAHI</t>
+  </si>
+  <si>
+    <t>This is english prompt</t>
   </si>
 </sst>
 </file>
@@ -564,9 +424,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35"/>
@@ -590,9 +450,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -613,9 +473,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74720F76-F09E-4599-AA7C-379CD9963F54}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -635,17 +495,35 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FBB029-B675-4E17-A37D-621363DDCB18}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added prompt edit and delete scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>OrgName</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>This is english prompt</t>
+  </si>
+  <si>
+    <t>This is updated english prompt</t>
   </si>
 </sst>
 </file>
@@ -523,7 +526,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added survey add edit and delete scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/sources/DriveHealthTestData.xlsx
+++ b/src/test/resources/sources/DriveHealthTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{27E43E09-A175-43B3-9CBC-A575CB3726B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9726D28D-6074-4713-869D-28050FF144B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrgData" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="MemberData" sheetId="3" r:id="rId3"/>
     <sheet name="StaffData" sheetId="4" r:id="rId4"/>
     <sheet name="prompt" sheetId="5" r:id="rId5"/>
+    <sheet name="survey" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <oleSize ref="A1:N5"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>OrgName</t>
   </si>
@@ -54,10 +55,13 @@
     <t>SLastVSAHI</t>
   </si>
   <si>
-    <t>This is english prompt</t>
-  </si>
-  <si>
     <t>This is updated english prompt</t>
+  </si>
+  <si>
+    <t>A Health Survey</t>
+  </si>
+  <si>
+    <t>A Updated Health Survey</t>
   </si>
 </sst>
 </file>
@@ -520,13 +524,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FBB029-B675-4E17-A37D-621363DDCB18}">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA524AD2-AFDD-4724-8865-012DDE270454}">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>